<commit_message>
Part 5 push 1
</commit_message>
<xml_diff>
--- a/Indiana Population Dataset.xlsx
+++ b/Indiana Population Dataset.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garobazarbachian/Desktop/NWU/MSDS 460/Requested-Group-Assignment-3-Integer-Programming-Example---Algorithmic-Redistricting-Spring-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FC536CF6-6A13-134C-A19E-9AF23500F30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBE507E-16FE-EC4A-9F6B-E707457B8D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_719" sheetId="2" r:id="rId1"/>
@@ -350,7 +350,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -859,11 +859,11 @@
     <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1239,11 +1239,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M83" sqref="M83"/>
+      <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,44 +1269,44 @@
       <c r="B3" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="7" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1334,7 +1334,7 @@
         <f>SUM(B7:G7)</f>
         <v>36068</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f>B7/H7</f>
         <v>0.97349451036930246</v>
       </c>
@@ -1365,7 +1365,7 @@
         <f t="shared" ref="H8:H71" si="0">SUM(B8:G8)</f>
         <v>391449</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <f t="shared" ref="I8:I71" si="1">B8/H8</f>
         <v>0.7849323922145669</v>
       </c>
@@ -1396,7 +1396,7 @@
         <f t="shared" si="0"/>
         <v>83540</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <f t="shared" si="1"/>
         <v>0.8662437155853483</v>
       </c>
@@ -1427,7 +1427,7 @@
         <f t="shared" si="0"/>
         <v>8719</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <f t="shared" si="1"/>
         <v>0.96215162289253353</v>
       </c>
@@ -1458,7 +1458,7 @@
         <f t="shared" si="0"/>
         <v>11919</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <f t="shared" si="1"/>
         <v>0.95712727577816936</v>
       </c>
@@ -1489,7 +1489,7 @@
         <f t="shared" si="0"/>
         <v>74164</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <f t="shared" si="1"/>
         <v>0.90736745590852708</v>
       </c>
@@ -1520,7 +1520,7 @@
         <f t="shared" si="0"/>
         <v>15570</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <f t="shared" si="1"/>
         <v>0.96281310211946047</v>
       </c>
@@ -1551,7 +1551,7 @@
         <f t="shared" si="0"/>
         <v>20555</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="6">
         <f t="shared" si="1"/>
         <v>0.96891267331549502</v>
       </c>
@@ -1582,7 +1582,7 @@
         <f t="shared" si="0"/>
         <v>37540</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <f t="shared" si="1"/>
         <v>0.9203249866808737</v>
       </c>
@@ -1613,7 +1613,7 @@
         <f t="shared" si="0"/>
         <v>124237</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <f t="shared" si="1"/>
         <v>0.86564389030643041</v>
       </c>
@@ -1644,7 +1644,7 @@
         <f t="shared" si="0"/>
         <v>26379</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <f t="shared" si="1"/>
         <v>0.9666022214640434</v>
       </c>
@@ -1675,7 +1675,7 @@
         <f t="shared" si="0"/>
         <v>32843</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <f t="shared" si="1"/>
         <v>0.96760344670097131</v>
       </c>
@@ -1706,7 +1706,7 @@
         <f t="shared" si="0"/>
         <v>10536</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <f t="shared" si="1"/>
         <v>0.96735003796507213</v>
       </c>
@@ -1737,7 +1737,7 @@
         <f t="shared" si="0"/>
         <v>33418</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="6">
         <f t="shared" si="1"/>
         <v>0.94742354419773778</v>
       </c>
@@ -1768,7 +1768,7 @@
         <f t="shared" si="0"/>
         <v>51138</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <f t="shared" si="1"/>
         <v>0.97058938558410579</v>
       </c>
@@ -1799,7 +1799,7 @@
         <f t="shared" si="0"/>
         <v>26416</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="6">
         <f t="shared" si="1"/>
         <v>0.96134918231374922</v>
       </c>
@@ -1830,7 +1830,7 @@
         <f t="shared" si="0"/>
         <v>43731</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="6">
         <f t="shared" si="1"/>
         <v>0.96967826027303283</v>
       </c>
@@ -1861,7 +1861,7 @@
         <f t="shared" si="0"/>
         <v>112031</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <f t="shared" si="1"/>
         <v>0.88090796297453389</v>
       </c>
@@ -1892,7 +1892,7 @@
         <f t="shared" si="0"/>
         <v>43632</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="6">
         <f t="shared" si="1"/>
         <v>0.96775302530253027</v>
       </c>
@@ -1923,7 +1923,7 @@
         <f t="shared" si="0"/>
         <v>206890</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="6">
         <f t="shared" si="1"/>
         <v>0.892938276378752</v>
       </c>
@@ -1954,7 +1954,7 @@
         <f t="shared" si="0"/>
         <v>23349</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="6">
         <f t="shared" si="1"/>
         <v>0.96376718489014523</v>
       </c>
@@ -1985,7 +1985,7 @@
         <f t="shared" si="0"/>
         <v>80714</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="6">
         <f t="shared" si="1"/>
         <v>0.89876601333102069</v>
       </c>
@@ -2016,7 +2016,7 @@
         <f t="shared" si="0"/>
         <v>16574</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="6">
         <f t="shared" si="1"/>
         <v>0.96814287438156144</v>
       </c>
@@ -2047,7 +2047,7 @@
         <f t="shared" si="0"/>
         <v>23028</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="6">
         <f t="shared" si="1"/>
         <v>0.97511724856696191</v>
       </c>
@@ -2078,7 +2078,7 @@
         <f t="shared" si="0"/>
         <v>20327</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="6">
         <f t="shared" si="1"/>
         <v>0.95951197914104391</v>
       </c>
@@ -2109,7 +2109,7 @@
         <f t="shared" si="0"/>
         <v>32993</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="6">
         <f t="shared" si="1"/>
         <v>0.93741096596247686</v>
       </c>
@@ -2140,7 +2140,7 @@
         <f t="shared" si="0"/>
         <v>66022</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="6">
         <f t="shared" si="1"/>
         <v>0.87837387537487499</v>
       </c>
@@ -2171,7 +2171,7 @@
         <f t="shared" si="0"/>
         <v>31006</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="6">
         <f t="shared" si="1"/>
         <v>0.97474682319551054</v>
       </c>
@@ -2202,7 +2202,7 @@
         <f t="shared" si="0"/>
         <v>364921</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="6">
         <f t="shared" si="1"/>
         <v>0.84967979370877533</v>
       </c>
@@ -2233,7 +2233,7 @@
         <f t="shared" si="0"/>
         <v>83070</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="6">
         <f t="shared" si="1"/>
         <v>0.92190923317683882</v>
       </c>
@@ -2264,7 +2264,7 @@
         <f t="shared" si="0"/>
         <v>39851</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I37" s="6">
         <f t="shared" si="1"/>
         <v>0.96592306341120671</v>
       </c>
@@ -2295,7 +2295,7 @@
         <f t="shared" si="0"/>
         <v>182534</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="6">
         <f t="shared" si="1"/>
         <v>0.82900719865887995</v>
       </c>
@@ -2326,7 +2326,7 @@
         <f t="shared" si="0"/>
         <v>48915</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I39" s="6">
         <f t="shared" si="1"/>
         <v>0.94825718082387811</v>
       </c>
@@ -2357,7 +2357,7 @@
         <f t="shared" si="0"/>
         <v>83574</v>
       </c>
-      <c r="I40" s="7">
+      <c r="I40" s="6">
         <f t="shared" si="1"/>
         <v>0.86730322827673678</v>
       </c>
@@ -2388,7 +2388,7 @@
         <f t="shared" si="0"/>
         <v>36834</v>
       </c>
-      <c r="I41" s="7">
+      <c r="I41" s="6">
         <f t="shared" si="1"/>
         <v>0.96421784221100071</v>
       </c>
@@ -2419,7 +2419,7 @@
         <f t="shared" si="0"/>
         <v>46300</v>
       </c>
-      <c r="I42" s="7">
+      <c r="I42" s="6">
         <f t="shared" si="1"/>
         <v>0.93479481641468687</v>
       </c>
@@ -2450,7 +2450,7 @@
         <f t="shared" si="0"/>
         <v>33281</v>
       </c>
-      <c r="I43" s="7">
+      <c r="I43" s="6">
         <f t="shared" si="1"/>
         <v>0.96968240137015116</v>
       </c>
@@ -2481,7 +2481,7 @@
         <f t="shared" si="0"/>
         <v>20198</v>
       </c>
-      <c r="I44" s="7">
+      <c r="I44" s="6">
         <f t="shared" si="1"/>
         <v>0.97306664026141199</v>
       </c>
@@ -2512,7 +2512,7 @@
         <f t="shared" si="0"/>
         <v>32946</v>
       </c>
-      <c r="I45" s="7">
+      <c r="I45" s="6">
         <f t="shared" si="1"/>
         <v>0.94846111819340739</v>
       </c>
@@ -2543,7 +2543,7 @@
         <f t="shared" si="0"/>
         <v>27536</v>
       </c>
-      <c r="I46" s="7">
+      <c r="I46" s="6">
         <f t="shared" si="1"/>
         <v>0.96786025566531086</v>
       </c>
@@ -2574,7 +2574,7 @@
         <f t="shared" si="0"/>
         <v>165782</v>
       </c>
-      <c r="I47" s="7">
+      <c r="I47" s="6">
         <f t="shared" si="1"/>
         <v>0.88457733650215342</v>
       </c>
@@ -2605,7 +2605,7 @@
         <f t="shared" si="0"/>
         <v>35789</v>
       </c>
-      <c r="I48" s="7">
+      <c r="I48" s="6">
         <f t="shared" si="1"/>
         <v>0.93847271508005248</v>
       </c>
@@ -2636,7 +2636,7 @@
         <f t="shared" si="0"/>
         <v>80826</v>
       </c>
-      <c r="I49" s="7">
+      <c r="I49" s="6">
         <f t="shared" si="1"/>
         <v>0.95125330957860099</v>
       </c>
@@ -2667,7 +2667,7 @@
         <f t="shared" si="0"/>
         <v>40866</v>
       </c>
-      <c r="I50" s="7">
+      <c r="I50" s="6">
         <f t="shared" si="1"/>
         <v>0.97917584299907012</v>
       </c>
@@ -2698,7 +2698,7 @@
         <f t="shared" si="0"/>
         <v>499689</v>
       </c>
-      <c r="I51" s="7">
+      <c r="I51" s="6">
         <f t="shared" si="1"/>
         <v>0.70933920898799052</v>
       </c>
@@ -2729,7 +2729,7 @@
         <f t="shared" si="0"/>
         <v>111675</v>
       </c>
-      <c r="I52" s="7">
+      <c r="I52" s="6">
         <f t="shared" si="1"/>
         <v>0.84658159838818003</v>
       </c>
@@ -2760,7 +2760,7 @@
         <f t="shared" si="0"/>
         <v>45222</v>
       </c>
-      <c r="I53" s="7">
+      <c r="I53" s="6">
         <f t="shared" si="1"/>
         <v>0.96691875635752511</v>
       </c>
@@ -2791,7 +2791,7 @@
         <f t="shared" si="0"/>
         <v>131744</v>
       </c>
-      <c r="I54" s="7">
+      <c r="I54" s="6">
         <f t="shared" si="1"/>
         <v>0.8791444012630556</v>
       </c>
@@ -2822,7 +2822,7 @@
         <f t="shared" si="0"/>
         <v>969466</v>
       </c>
-      <c r="I55" s="7">
+      <c r="I55" s="6">
         <f t="shared" si="1"/>
         <v>0.61879942153721734</v>
       </c>
@@ -2853,7 +2853,7 @@
         <f t="shared" si="0"/>
         <v>46332</v>
       </c>
-      <c r="I56" s="7">
+      <c r="I56" s="6">
         <f t="shared" si="1"/>
         <v>0.96244496244496247</v>
       </c>
@@ -2884,7 +2884,7 @@
         <f t="shared" si="0"/>
         <v>9803</v>
       </c>
-      <c r="I57" s="7">
+      <c r="I57" s="6">
         <f t="shared" si="1"/>
         <v>0.97133530551871872</v>
       </c>
@@ -2915,7 +2915,7 @@
         <f t="shared" si="0"/>
         <v>35674</v>
       </c>
-      <c r="I58" s="7">
+      <c r="I58" s="6">
         <f t="shared" si="1"/>
         <v>0.90993440600997921</v>
       </c>
@@ -2946,7 +2946,7 @@
         <f t="shared" si="0"/>
         <v>139745</v>
       </c>
-      <c r="I59" s="7">
+      <c r="I59" s="6">
         <f t="shared" si="1"/>
         <v>0.85885004830226486</v>
       </c>
@@ -2977,7 +2977,7 @@
         <f t="shared" si="0"/>
         <v>38273</v>
       </c>
-      <c r="I60" s="7">
+      <c r="I60" s="6">
         <f t="shared" si="1"/>
         <v>0.95879601808063131</v>
       </c>
@@ -3008,7 +3008,7 @@
         <f t="shared" si="0"/>
         <v>72236</v>
       </c>
-      <c r="I61" s="7">
+      <c r="I61" s="6">
         <f t="shared" si="1"/>
         <v>0.96611108034774906</v>
       </c>
@@ -3039,7 +3039,7 @@
         <f t="shared" si="0"/>
         <v>13823</v>
       </c>
-      <c r="I62" s="7">
+      <c r="I62" s="6">
         <f t="shared" si="1"/>
         <v>0.96180279244737032</v>
       </c>
@@ -3070,7 +3070,7 @@
         <f t="shared" si="0"/>
         <v>47367</v>
       </c>
-      <c r="I63" s="7">
+      <c r="I63" s="6">
         <f t="shared" si="1"/>
         <v>0.96320222940021538</v>
       </c>
@@ -3101,7 +3101,7 @@
         <f t="shared" si="0"/>
         <v>6114</v>
       </c>
-      <c r="I64" s="7">
+      <c r="I64" s="6">
         <f t="shared" si="1"/>
         <v>0.97055937193326791</v>
       </c>
@@ -3132,7 +3132,7 @@
         <f t="shared" si="0"/>
         <v>19623</v>
       </c>
-      <c r="I65" s="7">
+      <c r="I65" s="6">
         <f t="shared" si="1"/>
         <v>0.9597411201141518</v>
       </c>
@@ -3163,7 +3163,7 @@
         <f t="shared" si="0"/>
         <v>21482</v>
       </c>
-      <c r="I66" s="7">
+      <c r="I66" s="6">
         <f t="shared" si="1"/>
         <v>0.96806628805511596</v>
       </c>
@@ -3194,7 +3194,7 @@
         <f t="shared" si="0"/>
         <v>16369</v>
       </c>
-      <c r="I67" s="7">
+      <c r="I67" s="6">
         <f t="shared" si="1"/>
         <v>0.96004642922597594</v>
       </c>
@@ -3225,7 +3225,7 @@
         <f t="shared" si="0"/>
         <v>19183</v>
       </c>
-      <c r="I68" s="7">
+      <c r="I68" s="6">
         <f t="shared" si="1"/>
         <v>0.94328311525830166</v>
       </c>
@@ -3256,7 +3256,7 @@
         <f t="shared" si="0"/>
         <v>12168</v>
       </c>
-      <c r="I69" s="7">
+      <c r="I69" s="6">
         <f t="shared" si="1"/>
         <v>0.97000328731097962</v>
       </c>
@@ -3287,7 +3287,7 @@
         <f t="shared" si="0"/>
         <v>174791</v>
       </c>
-      <c r="I70" s="7">
+      <c r="I70" s="6">
         <f t="shared" si="1"/>
         <v>0.91217511199089196</v>
       </c>
@@ -3318,7 +3318,7 @@
         <f t="shared" si="0"/>
         <v>25063</v>
       </c>
-      <c r="I71" s="7">
+      <c r="I71" s="6">
         <f t="shared" si="1"/>
         <v>0.96580616845549216</v>
       </c>
@@ -3349,8 +3349,8 @@
         <f t="shared" ref="H72:H98" si="2">SUM(B72:G72)</f>
         <v>12485</v>
       </c>
-      <c r="I72" s="7">
-        <f t="shared" ref="I72:I100" si="3">B72/H72</f>
+      <c r="I72" s="6">
+        <f t="shared" ref="I72:I98" si="3">B72/H72</f>
         <v>0.96323588305967156</v>
       </c>
     </row>
@@ -3380,7 +3380,7 @@
         <f t="shared" si="2"/>
         <v>37301</v>
       </c>
-      <c r="I73" s="7">
+      <c r="I73" s="6">
         <f t="shared" si="3"/>
         <v>0.92981421409613685</v>
       </c>
@@ -3411,7 +3411,7 @@
         <f t="shared" si="2"/>
         <v>24437</v>
       </c>
-      <c r="I74" s="7">
+      <c r="I74" s="6">
         <f t="shared" si="3"/>
         <v>0.96619879690633059</v>
       </c>
@@ -3442,7 +3442,7 @@
         <f t="shared" si="2"/>
         <v>29087</v>
       </c>
-      <c r="I75" s="7">
+      <c r="I75" s="6">
         <f t="shared" si="3"/>
         <v>0.96881768487640529</v>
       </c>
@@ -3473,7 +3473,7 @@
         <f t="shared" si="2"/>
         <v>16673</v>
       </c>
-      <c r="I76" s="7">
+      <c r="I76" s="6">
         <f t="shared" si="3"/>
         <v>0.96803214778384217</v>
       </c>
@@ -3504,7 +3504,7 @@
         <f t="shared" si="2"/>
         <v>272234</v>
       </c>
-      <c r="I77" s="7">
+      <c r="I77" s="6">
         <f t="shared" si="3"/>
         <v>0.79149922493149272</v>
       </c>
@@ -3535,7 +3535,7 @@
         <f t="shared" si="2"/>
         <v>24588</v>
       </c>
-      <c r="I78" s="7">
+      <c r="I78" s="6">
         <f t="shared" si="3"/>
         <v>0.96660972832275904</v>
       </c>
@@ -3566,7 +3566,7 @@
         <f t="shared" si="2"/>
         <v>44991</v>
       </c>
-      <c r="I79" s="7">
+      <c r="I79" s="6">
         <f t="shared" si="3"/>
         <v>0.95401302482718764</v>
       </c>
@@ -3597,7 +3597,7 @@
         <f t="shared" si="2"/>
         <v>19967</v>
       </c>
-      <c r="I80" s="7">
+      <c r="I80" s="6">
         <f t="shared" si="3"/>
         <v>0.96934942655381384</v>
       </c>
@@ -3628,7 +3628,7 @@
         <f t="shared" si="2"/>
         <v>23258</v>
       </c>
-      <c r="I81" s="7">
+      <c r="I81" s="6">
         <f t="shared" si="3"/>
         <v>0.96805400292372512</v>
       </c>
@@ -3659,7 +3659,7 @@
         <f t="shared" si="2"/>
         <v>34725</v>
       </c>
-      <c r="I82" s="7">
+      <c r="I82" s="6">
         <f t="shared" si="3"/>
         <v>0.9640028797696184</v>
       </c>
@@ -3690,7 +3690,7 @@
         <f t="shared" si="2"/>
         <v>20670</v>
       </c>
-      <c r="I83" s="7">
+      <c r="I83" s="6">
         <f t="shared" si="3"/>
         <v>0.92723754233188194</v>
       </c>
@@ -3721,7 +3721,7 @@
         <f t="shared" si="2"/>
         <v>10006</v>
       </c>
-      <c r="I84" s="7">
+      <c r="I84" s="6">
         <f t="shared" si="3"/>
         <v>0.96512092744353384</v>
       </c>
@@ -3752,7 +3752,7 @@
         <f t="shared" si="2"/>
         <v>188717</v>
       </c>
-      <c r="I85" s="7">
+      <c r="I85" s="6">
         <f t="shared" si="3"/>
         <v>0.82217818214575267</v>
       </c>
@@ -3783,7 +3783,7 @@
         <f t="shared" si="2"/>
         <v>15361</v>
       </c>
-      <c r="I86" s="7">
+      <c r="I86" s="6">
         <f t="shared" si="3"/>
         <v>0.96146084239307339</v>
       </c>
@@ -3814,7 +3814,7 @@
         <f t="shared" si="2"/>
         <v>6952</v>
       </c>
-      <c r="I87" s="7">
+      <c r="I87" s="6">
         <f t="shared" si="3"/>
         <v>0.9630322209436134</v>
       </c>
@@ -3845,7 +3845,7 @@
         <f t="shared" si="2"/>
         <v>179744</v>
       </c>
-      <c r="I88" s="7">
+      <c r="I88" s="6">
         <f t="shared" si="3"/>
         <v>0.84495727256542641</v>
       </c>
@@ -3876,7 +3876,7 @@
         <f t="shared" si="2"/>
         <v>15451</v>
       </c>
-      <c r="I89" s="7">
+      <c r="I89" s="6">
         <f t="shared" si="3"/>
         <v>0.96912821176622876</v>
       </c>
@@ -3907,7 +3907,7 @@
         <f t="shared" si="2"/>
         <v>106006</v>
       </c>
-      <c r="I90" s="7">
+      <c r="I90" s="6">
         <f t="shared" si="3"/>
         <v>0.87731826500386767</v>
       </c>
@@ -3938,7 +3938,7 @@
         <f t="shared" si="2"/>
         <v>30828</v>
       </c>
-      <c r="I91" s="7">
+      <c r="I91" s="6">
         <f t="shared" si="3"/>
         <v>0.9631828208122486</v>
       </c>
@@ -3969,7 +3969,7 @@
         <f t="shared" si="2"/>
         <v>8461</v>
       </c>
-      <c r="I92" s="7">
+      <c r="I92" s="6">
         <f t="shared" si="3"/>
         <v>0.97340739865264159</v>
       </c>
@@ -4000,7 +4000,7 @@
         <f t="shared" si="2"/>
         <v>65185</v>
       </c>
-      <c r="I93" s="7">
+      <c r="I93" s="6">
         <f t="shared" si="3"/>
         <v>0.92849581959039651</v>
       </c>
@@ -4031,7 +4031,7 @@
         <f t="shared" si="2"/>
         <v>28224</v>
       </c>
-      <c r="I94" s="7">
+      <c r="I94" s="6">
         <f t="shared" si="3"/>
         <v>0.97388747165532885</v>
       </c>
@@ -4062,7 +4062,7 @@
         <f t="shared" si="2"/>
         <v>66273</v>
       </c>
-      <c r="I95" s="7">
+      <c r="I95" s="6">
         <f t="shared" si="3"/>
         <v>0.89893320054924331</v>
       </c>
@@ -4093,7 +4093,7 @@
         <f t="shared" si="2"/>
         <v>28335</v>
       </c>
-      <c r="I96" s="7">
+      <c r="I96" s="6">
         <f t="shared" si="3"/>
         <v>0.96393153343920945</v>
       </c>
@@ -4124,7 +4124,7 @@
         <f t="shared" si="2"/>
         <v>24598</v>
       </c>
-      <c r="I97" s="7">
+      <c r="I97" s="6">
         <f t="shared" si="3"/>
         <v>0.95877713635254902</v>
       </c>
@@ -4155,7 +4155,7 @@
         <f t="shared" si="2"/>
         <v>34627</v>
       </c>
-      <c r="I98" s="7">
+      <c r="I98" s="6">
         <f t="shared" si="3"/>
         <v>0.96722210991422874</v>
       </c>
@@ -4172,16 +4172,16 @@
         <f>SUM(H7:H98)</f>
         <v>6833037</v>
       </c>
-      <c r="I99" s="7">
+      <c r="I99" s="6">
         <f>B99/H99</f>
         <v>0.83958918998975129</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A100" s="6" t="s">
+      <c r="A100" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I100" s="7"/>
+      <c r="I100" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>